<commit_message>
newi input data record
</commit_message>
<xml_diff>
--- a/tugas_akhir/dokumenTA/data-pengujianbsf-1.xlsx
+++ b/tugas_akhir/dokumenTA/data-pengujianbsf-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benny\OneDrive\Documents\PlatformIO\Projects\Project-Tugas-Akhir\tugas_akhir\dokumenTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97DD7C2-5766-474C-99EB-1E22A76C3B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E1D8D2-9930-4213-B00C-0BDC633744B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sensor Data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>tanggal</t>
   </si>
@@ -104,9 +104,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                       </t>
   </si>
 </sst>
 </file>
@@ -470,6 +467,12 @@
                 <c:pt idx="15">
                   <c:v>36.1</c:v>
                 </c:pt>
+                <c:pt idx="16">
+                  <c:v>28.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>34.799999999999997</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -672,6 +675,12 @@
                   <c:v>33.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>33.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>33.700000000000003</c:v>
                 </c:pt>
               </c:numCache>
@@ -911,6 +920,12 @@
                       <c:pt idx="15">
                         <c:v>46</c:v>
                       </c:pt>
+                      <c:pt idx="16">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>55</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -1135,6 +1150,12 @@
                       <c:pt idx="15">
                         <c:v>52</c:v>
                       </c:pt>
+                      <c:pt idx="16">
+                        <c:v>67</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>62</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -1359,6 +1380,12 @@
                       <c:pt idx="15">
                         <c:v>6834</c:v>
                       </c:pt>
+                      <c:pt idx="16">
+                        <c:v>3604</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>8485</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -1582,6 +1609,12 @@
                       </c:pt>
                       <c:pt idx="15">
                         <c:v>15110</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>9220</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>22850</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1814,10 +1847,10 @@
                         <c:v>2.3999999999999986</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-1.3999999999999986</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>1.0999999999999943</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -2056,10 +2089,10 @@
                         <c:v>-6</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-3</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>-7</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -2298,10 +2331,10 @@
                         <c:v>-8276</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-5616</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>-14365</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -2540,10 +2573,10 @@
                         <c:v>7.121661721068244E-2</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-4.745762711864402E-2</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>3.2640949554895972E-2</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -2782,10 +2815,10 @@
                         <c:v>-0.11538461538461539</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-4.4776119402985072E-2</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>-0.11290322580645161</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -3024,10 +3057,10 @@
                         <c:v>-0.54771674387822633</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-0.60911062906724511</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>-0.62866520787746172</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -3523,6 +3556,12 @@
                 <c:pt idx="15">
                   <c:v>46</c:v>
                 </c:pt>
+                <c:pt idx="16">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>55</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -3729,6 +3768,12 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -3968,6 +4013,12 @@
                       <c:pt idx="15">
                         <c:v>36.1</c:v>
                       </c:pt>
+                      <c:pt idx="16">
+                        <c:v>28.1</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>34.799999999999997</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4192,6 +4243,12 @@
                       <c:pt idx="15">
                         <c:v>33.700000000000003</c:v>
                       </c:pt>
+                      <c:pt idx="16">
+                        <c:v>29.5</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>33.700000000000003</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4416,6 +4473,12 @@
                       <c:pt idx="15">
                         <c:v>6834</c:v>
                       </c:pt>
+                      <c:pt idx="16">
+                        <c:v>3604</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>8485</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4639,6 +4702,12 @@
                       </c:pt>
                       <c:pt idx="15">
                         <c:v>15110</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>9220</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>22850</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4871,10 +4940,10 @@
                         <c:v>2.3999999999999986</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-1.3999999999999986</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>1.0999999999999943</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -5113,10 +5182,10 @@
                         <c:v>-6</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-3</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>-7</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -5355,10 +5424,10 @@
                         <c:v>-8276</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-5616</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>-14365</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -5597,10 +5666,10 @@
                         <c:v>7.121661721068244E-2</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-4.745762711864402E-2</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>3.2640949554895972E-2</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -5839,10 +5908,10 @@
                         <c:v>-0.11538461538461539</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-4.4776119402985072E-2</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>-0.11290322580645161</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -6081,10 +6150,10 @@
                         <c:v>-0.54771674387822633</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-0.60911062906724511</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>-0.62866520787746172</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -6575,6 +6644,12 @@
                 <c:pt idx="15">
                   <c:v>6834</c:v>
                 </c:pt>
+                <c:pt idx="16">
+                  <c:v>3604</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8485</c:v>
+                </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
@@ -6781,6 +6856,12 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>15110</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9220</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>22850</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -7020,6 +7101,12 @@
                       <c:pt idx="15">
                         <c:v>36.1</c:v>
                       </c:pt>
+                      <c:pt idx="16">
+                        <c:v>28.1</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>34.799999999999997</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -7244,6 +7331,12 @@
                       <c:pt idx="15">
                         <c:v>33.700000000000003</c:v>
                       </c:pt>
+                      <c:pt idx="16">
+                        <c:v>29.5</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>33.700000000000003</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -7468,6 +7561,12 @@
                       <c:pt idx="15">
                         <c:v>46</c:v>
                       </c:pt>
+                      <c:pt idx="16">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>55</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -7691,6 +7790,12 @@
                       </c:pt>
                       <c:pt idx="15">
                         <c:v>52</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>67</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>62</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -7923,10 +8028,10 @@
                         <c:v>2.3999999999999986</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-1.3999999999999986</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>1.0999999999999943</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -8165,10 +8270,10 @@
                         <c:v>-6</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-3</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>-7</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -8407,10 +8512,10 @@
                         <c:v>-8276</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-5616</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>-14365</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -8649,10 +8754,10 @@
                         <c:v>7.121661721068244E-2</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-4.745762711864402E-2</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>3.2640949554895972E-2</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -8891,10 +8996,10 @@
                         <c:v>-0.11538461538461539</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-4.4776119402985072E-2</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>-0.11290322580645161</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -9133,10 +9238,10 @@
                         <c:v>-0.54771674387822633</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-0.60911062906724511</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>-0.62866520787746172</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -9639,10 +9744,10 @@
                   <c:v>7.121661721068244E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>-4.745762711864402E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>3.2640949554895972E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -9864,10 +9969,10 @@
                   <c:v>-0.11538461538461539</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>-4.4776119402985072E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>-0.11290322580645161</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -10089,10 +10194,10 @@
                   <c:v>-0.54771674387822633</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>-0.60911062906724511</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>-0.62866520787746172</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -10338,6 +10443,12 @@
                       <c:pt idx="15">
                         <c:v>36.1</c:v>
                       </c:pt>
+                      <c:pt idx="16">
+                        <c:v>28.1</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>34.799999999999997</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -10562,6 +10673,12 @@
                       <c:pt idx="15">
                         <c:v>33.700000000000003</c:v>
                       </c:pt>
+                      <c:pt idx="16">
+                        <c:v>29.5</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>33.700000000000003</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -10786,6 +10903,12 @@
                       <c:pt idx="15">
                         <c:v>46</c:v>
                       </c:pt>
+                      <c:pt idx="16">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>55</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -11010,6 +11133,12 @@
                       <c:pt idx="15">
                         <c:v>52</c:v>
                       </c:pt>
+                      <c:pt idx="16">
+                        <c:v>67</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>62</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -11234,6 +11363,12 @@
                       <c:pt idx="15">
                         <c:v>6834</c:v>
                       </c:pt>
+                      <c:pt idx="16">
+                        <c:v>3604</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>8485</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -11457,6 +11592,12 @@
                       </c:pt>
                       <c:pt idx="15">
                         <c:v>15110</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>9220</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>22850</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -11689,10 +11830,10 @@
                         <c:v>2.3999999999999986</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-1.3999999999999986</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>1.0999999999999943</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -11931,10 +12072,10 @@
                         <c:v>-6</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-3</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>-7</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -12173,10 +12314,10 @@
                         <c:v>-8276</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0</c:v>
+                        <c:v>-5616</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0</c:v>
+                        <c:v>-14365</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>0</c:v>
@@ -12666,7 +12807,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16048,8 +16192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="86" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -16961,38 +17105,50 @@
       <c r="B18" s="2">
         <v>0.375</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="C18" s="3">
+        <v>28.1</v>
+      </c>
+      <c r="D18" s="3">
+        <v>29.5</v>
+      </c>
+      <c r="E18" s="3">
+        <v>64</v>
+      </c>
+      <c r="F18" s="3">
+        <v>67</v>
+      </c>
+      <c r="G18" s="3">
+        <v>3604</v>
+      </c>
+      <c r="H18" s="3">
+        <v>9220</v>
+      </c>
       <c r="I18" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1.3999999999999986</v>
       </c>
       <c r="J18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="K18">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L18" s="5" t="e">
+        <v>-5616</v>
+      </c>
+      <c r="L18" s="5">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M18" s="5" t="e">
+        <v>-4.745762711864402E-2</v>
+      </c>
+      <c r="M18" s="5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N18" s="5" t="e">
+        <v>-4.4776119402985072E-2</v>
+      </c>
+      <c r="N18" s="5">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O18" t="s">
-        <v>23</v>
+        <v>-0.60911062906724511</v>
+      </c>
+      <c r="O18">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -17000,35 +17156,50 @@
       <c r="B19" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="C19" s="3">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="D19" s="3">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="E19" s="3">
+        <v>55</v>
+      </c>
+      <c r="F19" s="3">
+        <v>62</v>
+      </c>
+      <c r="G19" s="3">
+        <v>8485</v>
+      </c>
+      <c r="H19" s="3">
+        <v>22850</v>
+      </c>
       <c r="I19" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.0999999999999943</v>
       </c>
       <c r="J19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-7</v>
       </c>
       <c r="K19">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L19" s="5" t="e">
+        <v>-14365</v>
+      </c>
+      <c r="L19" s="5">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M19" s="5" t="e">
+        <v>3.2640949554895972E-2</v>
+      </c>
+      <c r="M19" s="5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N19" s="5" t="e">
+        <v>-0.11290322580645161</v>
+      </c>
+      <c r="N19" s="5">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>-0.62866520787746172</v>
+      </c>
+      <c r="O19">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -17125,7 +17296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302D2EB0-8602-40F5-B743-D70D0FC2E10C}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
backup tahap akhir - 1
</commit_message>
<xml_diff>
--- a/tugas_akhir/dokumenTA/data-pengujianbsf-1.xlsx
+++ b/tugas_akhir/dokumenTA/data-pengujianbsf-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benny\OneDrive\Documents\PlatformIO\Projects\Project-Tugas-Akhir\tugas_akhir\dokumenTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD97DB98-C6A4-4054-8E43-D770DFE05C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5945066B-04E8-4ACE-9D08-6E6EDCE9B631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,34 +17,32 @@
     <sheet name="Produksi Telur Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Sensor Data'!#REF!</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Sensor Data'!#REF!</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Sensor Data'!$F$2:$F$21</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'Sensor Data'!$G$1</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'Sensor Data'!$G$2:$G$21</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'Sensor Data'!$H$1</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'Sensor Data'!$H$2:$H$21</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'Sensor Data'!$I$1</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'Sensor Data'!$I$2:$I$21</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'Sensor Data'!$J$1</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'Sensor Data'!$J$2:$J$21</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'Sensor Data'!$K$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Sensor Data'!$A$2:$B$21</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">'Sensor Data'!$K$2:$K$21</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">'Sensor Data'!$L$1</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">'Sensor Data'!$L$2:$L$21</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">'Sensor Data'!$M$1</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">'Sensor Data'!$M$2:$M$21</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">'Sensor Data'!$N$1</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">'Sensor Data'!$N$2:$N$21</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">'Sensor Data'!$P$18</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Sensor Data'!$C$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Sensor Data'!$C$2:$C$21</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Sensor Data'!$D$1</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Sensor Data'!$D$2:$D$21</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Sensor Data'!$E$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Sensor Data'!$E$2:$E$21</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Sensor Data'!$F$1</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Sensor Data'!$A$2:$B$21</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Sensor Data'!$C$1</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'Sensor Data'!$G$2:$G$21</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'Sensor Data'!$H$1</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'Sensor Data'!$H$2:$H$21</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'Sensor Data'!$I$1</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'Sensor Data'!$I$2:$I$21</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'Sensor Data'!$J$1</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'Sensor Data'!$J$2:$J$21</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'Sensor Data'!$K$1</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'Sensor Data'!$K$2:$K$21</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'Sensor Data'!$L$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Sensor Data'!$C$2:$C$21</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'Sensor Data'!$L$2:$L$21</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'Sensor Data'!$M$1</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'Sensor Data'!$M$2:$M$21</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'Sensor Data'!$N$1</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">'Sensor Data'!$N$2:$N$21</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">'Sensor Data'!$P$18</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Sensor Data'!$D$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Sensor Data'!$D$2:$D$21</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Sensor Data'!$E$1</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Sensor Data'!$E$2:$E$21</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Sensor Data'!$F$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'Sensor Data'!$F$2:$F$21</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'Sensor Data'!$G$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
   <si>
     <t>tanggal</t>
   </si>
@@ -219,6 +217,15 @@
   <si>
     <t>avg-alat ukur-lx</t>
   </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
 </sst>
 </file>
 
@@ -226,7 +233,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-13809]hh:mm;@"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -276,7 +283,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -289,7 +296,9 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5012,6 +5021,62 @@
             </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'Sensor Data'!$P$17:$R$17</c:f>
@@ -5054,8 +5119,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -7782,7 +7848,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -7992,7 +8058,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -26354,6 +26420,11 @@
             <c:idx val="0"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-6632-4DEB-8E31-FF5D502F87D5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -27016,7 +27087,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Sensor Data'!$Q$17</c15:sqref>
@@ -27046,7 +27117,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Sensor Data'!$Q$18</c15:sqref>
@@ -27062,7 +27133,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000F-29BF-4A7C-83CE-DAD531E83558}"/>
                   </c:ext>
@@ -27075,7 +27146,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Sensor Data'!$R$17</c15:sqref>
@@ -27105,7 +27176,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Sensor Data'!$R$18</c15:sqref>
@@ -27121,7 +27192,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000010-29BF-4A7C-83CE-DAD531E83558}"/>
                   </c:ext>
@@ -27134,7 +27205,7 @@
                 <c:order val="6"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Sensor Data'!$P$8</c15:sqref>
@@ -27161,7 +27232,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Sensor Data'!$P$9</c15:sqref>
@@ -27177,7 +27248,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000008-E290-404F-9DDE-63577070BE5B}"/>
                   </c:ext>
@@ -27190,7 +27261,7 @@
                 <c:order val="7"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Sensor Data'!$Q$8</c15:sqref>
@@ -27217,7 +27288,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Sensor Data'!$Q$9</c15:sqref>
@@ -27233,7 +27304,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-E290-404F-9DDE-63577070BE5B}"/>
                   </c:ext>
@@ -27246,7 +27317,7 @@
                 <c:order val="8"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Sensor Data'!$R$8</c15:sqref>
@@ -27273,7 +27344,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Sensor Data'!$R$9</c15:sqref>
@@ -27289,7 +27360,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000A-E290-404F-9DDE-63577070BE5B}"/>
                   </c:ext>
@@ -27461,103 +27532,103 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.0</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
         <cx:f>_xlchart.v1.2</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
         <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
-    <cx:data id="1">
+    <cx:data id="2">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
         <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
-    <cx:data id="2">
+    <cx:data id="3">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
         <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
-    <cx:data id="3">
+    <cx:data id="4">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
         <cx:f>_xlchart.v1.10</cx:f>
       </cx:numDim>
     </cx:data>
-    <cx:data id="4">
+    <cx:data id="5">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
         <cx:f>_xlchart.v1.12</cx:f>
       </cx:numDim>
     </cx:data>
-    <cx:data id="5">
+    <cx:data id="6">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
         <cx:f>_xlchart.v1.14</cx:f>
       </cx:numDim>
     </cx:data>
-    <cx:data id="6">
+    <cx:data id="7">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
         <cx:f>_xlchart.v1.16</cx:f>
       </cx:numDim>
     </cx:data>
-    <cx:data id="7">
+    <cx:data id="8">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
         <cx:f>_xlchart.v1.18</cx:f>
       </cx:numDim>
     </cx:data>
-    <cx:data id="8">
+    <cx:data id="9">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
         <cx:f>_xlchart.v1.20</cx:f>
       </cx:numDim>
     </cx:data>
-    <cx:data id="9">
+    <cx:data id="10">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
         <cx:f>_xlchart.v1.22</cx:f>
       </cx:numDim>
     </cx:data>
-    <cx:data id="10">
+    <cx:data id="11">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
         <cx:f>_xlchart.v1.24</cx:f>
       </cx:numDim>
     </cx:data>
-    <cx:data id="11">
-      <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.2</cx:f>
-      </cx:strDim>
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.26</cx:f>
-      </cx:numDim>
-    </cx:data>
     <cx:data id="12">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.27</cx:f>
+        <cx:f>_xlchart.v1.25</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -27688,7 +27759,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{9580C7CB-6903-4D6F-BC1C-86D62367110E}" formatIdx="0">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.3</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>dht11-temp</cx:v>
             </cx:txData>
           </cx:tx>
@@ -27700,7 +27771,7 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{78B99813-F2FD-4F4F-9F3B-65DA602F2917}" formatIdx="1">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.5</cx:f>
+              <cx:f>_xlchart.v1.3</cx:f>
               <cx:v>alat ukur-temp</cx:v>
             </cx:txData>
           </cx:tx>
@@ -27712,7 +27783,7 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{AD8FB238-4537-4A89-9739-2B54DFD51478}" formatIdx="2">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.7</cx:f>
+              <cx:f>_xlchart.v1.5</cx:f>
               <cx:v>dht11-humi</cx:v>
             </cx:txData>
           </cx:tx>
@@ -27724,7 +27795,7 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{1ADAA32C-526D-4F3D-A848-098FC25DA4FD}" formatIdx="3">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.9</cx:f>
+              <cx:f>_xlchart.v1.7</cx:f>
               <cx:v>alat ukur-humi</cx:v>
             </cx:txData>
           </cx:tx>
@@ -27736,7 +27807,7 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{29D1B0F3-1C35-489C-813C-AC5DA2C7B373}" formatIdx="4">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.11</cx:f>
+              <cx:f>_xlchart.v1.9</cx:f>
               <cx:v>bh1750-lx</cx:v>
             </cx:txData>
           </cx:tx>
@@ -27748,7 +27819,7 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{7A577398-F204-41A4-A604-CC5230D57045}" formatIdx="5">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.13</cx:f>
+              <cx:f>_xlchart.v1.11</cx:f>
               <cx:v>alat ukur-lx</cx:v>
             </cx:txData>
           </cx:tx>
@@ -27760,7 +27831,7 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{0EA38A03-2142-4B66-AD7A-3334C088D14F}" formatIdx="6">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.15</cx:f>
+              <cx:f>_xlchart.v1.13</cx:f>
               <cx:v>delta-temp</cx:v>
             </cx:txData>
           </cx:tx>
@@ -27772,7 +27843,7 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{936D1409-A4A0-40E6-90BD-45632CC323D7}" formatIdx="7">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.17</cx:f>
+              <cx:f>_xlchart.v1.15</cx:f>
               <cx:v>delta-humi</cx:v>
             </cx:txData>
           </cx:tx>
@@ -27784,7 +27855,7 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{F0BE6223-D54B-4DEC-B87C-A7692BEC2B50}" formatIdx="8">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.19</cx:f>
+              <cx:f>_xlchart.v1.17</cx:f>
               <cx:v>delta-lx</cx:v>
             </cx:txData>
           </cx:tx>
@@ -27796,7 +27867,7 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{DC9BE140-525D-464E-A73D-05D6045611F2}" formatIdx="9">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.21</cx:f>
+              <cx:f>_xlchart.v1.19</cx:f>
               <cx:v>percent-temp</cx:v>
             </cx:txData>
           </cx:tx>
@@ -27808,7 +27879,7 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{ED700A51-24FC-4D6D-9260-C4E7D9BD573F}" formatIdx="10">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.23</cx:f>
+              <cx:f>_xlchart.v1.21</cx:f>
               <cx:v>percent-humi</cx:v>
             </cx:txData>
           </cx:tx>
@@ -27820,7 +27891,7 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{0FB62097-8A96-4586-BB8E-2507F501DDDE}" formatIdx="11">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.25</cx:f>
+              <cx:f>_xlchart.v1.23</cx:f>
               <cx:v>percent-lx</cx:v>
             </cx:txData>
           </cx:tx>
@@ -27832,7 +27903,7 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{AB1DA2D7-99D1-4719-9B48-D37E506BC2AD}" formatIdx="13">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.23</cx:f>
+              <cx:f>_xlchart.v1.21</cx:f>
               <cx:v>percent-humi</cx:v>
             </cx:txData>
           </cx:tx>
@@ -37683,15 +37754,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>91802</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>11305</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>15658</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>396602</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>11305</xdr:rowOff>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>15659</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -37727,8 +37798,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="91802" y="4217545"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="0" y="4827144"/>
+              <a:ext cx="4572000" cy="2775858"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -37761,15 +37832,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>91802</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>2870</xdr:rowOff>
+      <xdr:colOff>24311</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>137853</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>396602</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>2870</xdr:rowOff>
+      <xdr:colOff>329111</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>137853</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -37797,15 +37868,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>501927</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>13637</xdr:rowOff>
+      <xdr:colOff>477978</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>199056</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>13637</xdr:rowOff>
+      <xdr:colOff>175107</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>574</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -37833,15 +37904,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>512988</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>181611</xdr:rowOff>
+      <xdr:colOff>475976</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>208188</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>181611</xdr:rowOff>
+      <xdr:colOff>171176</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -37869,15 +37940,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>356887</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>2893</xdr:rowOff>
+      <xdr:colOff>317699</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>31195</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>67520</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>180372</xdr:rowOff>
+      <xdr:colOff>28332</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>25795</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -37905,15 +37976,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>390714</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>59336</xdr:rowOff>
+      <xdr:colOff>329754</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>35388</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>85913</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>59337</xdr:rowOff>
+      <xdr:colOff>24953</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>35389</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -37941,15 +38012,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>107180</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>6174</xdr:rowOff>
+      <xdr:colOff>22271</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>115031</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>413751</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>6174</xdr:rowOff>
+      <xdr:colOff>328842</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>115031</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -37977,15 +38048,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>585644</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>183383</xdr:rowOff>
+      <xdr:colOff>472433</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>118069</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>280844</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>183383</xdr:rowOff>
+      <xdr:colOff>167633</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>118069</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -38013,15 +38084,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>428685</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>100263</xdr:rowOff>
+      <xdr:colOff>304588</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>135097</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>121880</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>100263</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>607383</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>135097</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -38049,15 +38120,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>445872</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>177013</xdr:rowOff>
+      <xdr:colOff>343547</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>102991</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>139067</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>177012</xdr:rowOff>
+      <xdr:colOff>36742</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>102989</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -38641,10 +38712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V23"/>
+  <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="96" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="AO16" sqref="AO16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -39960,7 +40031,91 @@
     </row>
     <row r="23" spans="1:22">
       <c r="E23" s="3"/>
-      <c r="H23" s="3"/>
+      <c r="H23" t="s">
+        <v>51</v>
+      </c>
+      <c r="I23" s="9">
+        <f>AVERAGE(I2:I21)</f>
+        <v>-0.12000000000000011</v>
+      </c>
+      <c r="J23">
+        <f>AVERAGE(J2:J21)</f>
+        <v>-3.55</v>
+      </c>
+      <c r="K23">
+        <f>AVERAGE(K2:K21)</f>
+        <v>-9173.2000000000007</v>
+      </c>
+      <c r="L23" s="5">
+        <f>AVERAGE(L2:L21)</f>
+        <v>-3.5288000624746152E-3</v>
+      </c>
+      <c r="M23" s="10">
+        <f>AVERAGE(M2:M21)</f>
+        <v>-5.2595144374515526E-2</v>
+      </c>
+      <c r="N23" s="10">
+        <f>AVERAGE(N2:N21)</f>
+        <v>-0.60928632929819393</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22">
+      <c r="H24" t="s">
+        <v>52</v>
+      </c>
+      <c r="I24" s="9">
+        <f>MAX(I2:I21)</f>
+        <v>2.3999999999999986</v>
+      </c>
+      <c r="J24">
+        <f>MAX(J2:J21)</f>
+        <v>3</v>
+      </c>
+      <c r="K24">
+        <f>MAX(K2:K21)</f>
+        <v>-2363</v>
+      </c>
+      <c r="L24" s="10">
+        <f>MAX(L2:L21)</f>
+        <v>7.2847682119205281E-2</v>
+      </c>
+      <c r="M24" s="10">
+        <f>MAX(M2:M21)</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="N24" s="10">
+        <f>MAX(N2:N21)</f>
+        <v>-0.43783583472299425</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22">
+      <c r="H25" t="s">
+        <v>53</v>
+      </c>
+      <c r="I25" s="9">
+        <f>MIN(I2:I21)</f>
+        <v>-1.6999999999999957</v>
+      </c>
+      <c r="J25">
+        <f>MIN(J2:J21)</f>
+        <v>-13</v>
+      </c>
+      <c r="K25">
+        <f>MIN(K2:K21)</f>
+        <v>-29165</v>
+      </c>
+      <c r="L25" s="10">
+        <f>MIN(L2:L21)</f>
+        <v>-4.871060171919759E-2</v>
+      </c>
+      <c r="M25" s="10">
+        <f>MIN(M2:M21)</f>
+        <v>-0.17808219178082191</v>
+      </c>
+      <c r="N25" s="10">
+        <f>MIN(N2:N21)</f>
+        <v>-0.64441883437602898</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
sisa bab 5 dan abstrak
</commit_message>
<xml_diff>
--- a/tugas_akhir/dokumenTA/data-pengujianbsf-1.xlsx
+++ b/tugas_akhir/dokumenTA/data-pengujianbsf-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benny\OneDrive\Documents\PlatformIO\Projects\Project-Tugas-Akhir\tugas_akhir\dokumenTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5945066B-04E8-4ACE-9D08-6E6EDCE9B631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D51351-5D06-4CB3-8ED8-E33422A5D91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6203,6 +6203,1885 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Indeks Cuaca</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sensor Data'!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cuaca</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="FF0000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Sensor Data'!$A$2:$B$21</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="20"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>09:00</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>14:00</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>09:00</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>14:00</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>09:00</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>14:00</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>09:00</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>14:00</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>09:00</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>14:00</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>09:00</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>14:00</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>09:00</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>14:00</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>09:00</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>14:00</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>09:00</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>14:00</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>09:00</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>14:00</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>05-Jun</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>06-Jun</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>07-Jun</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>08-Jun</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>09-Jun</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>12-Jun</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>13-Jun</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>14-Jun</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>15-Jun</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>16-Jun</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sensor Data'!$O$2:$O$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DA27-466D-8954-5025739127F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1481513888"/>
+        <c:axId val="1481514368"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1481513888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="high"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1481514368"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1481514368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1481513888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Indeks Cuaca</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Produksi Telur Data'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cuaca</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent4">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Produksi Telur Data'!$A$2:$B$7</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>09:00</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>09:00</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>09:00</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>09:00</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>09:00</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>09:00</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>05-Jun</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>07-Jun</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>09-Jun</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>12-Jun</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>14-Jun</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>16-Jun</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Produksi Telur Data'!$F$2:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3FDB-4687-A9DE-BDDA83D550B4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="r"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1846123872"/>
+        <c:axId val="1846133952"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Produksi Telur Data'!$C$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>dht11-temp</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="22225" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:glow rad="139700">
+                      <a:schemeClr val="accent1">
+                        <a:satMod val="175000"/>
+                        <a:alpha val="14000"/>
+                      </a:schemeClr>
+                    </a:glow>
+                  </a:effectLst>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="4"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1">
+                        <a:lumMod val="60000"/>
+                        <a:lumOff val="40000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst>
+                      <a:glow rad="63500">
+                        <a:schemeClr val="accent1">
+                          <a:satMod val="175000"/>
+                          <a:alpha val="25000"/>
+                        </a:schemeClr>
+                      </a:glow>
+                    </a:effectLst>
+                  </c:spPr>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="lt1">
+                              <a:lumMod val="75000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="r"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="lt1">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Produksi Telur Data'!$A$2:$B$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="6"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>05-Jun</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>07-Jun</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>09-Jun</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>12-Jun</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>14-Jun</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>16-Jun</c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Produksi Telur Data'!$C$2:$C$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>30.7</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>31.9</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>29.2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>31.2</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>31.6</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>30.5</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-3FDB-4687-A9DE-BDDA83D550B4}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Produksi Telur Data'!$D$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>dht11-humi</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="22225" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:glow rad="139700">
+                      <a:schemeClr val="accent2">
+                        <a:satMod val="175000"/>
+                        <a:alpha val="14000"/>
+                      </a:schemeClr>
+                    </a:glow>
+                  </a:effectLst>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="4"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2">
+                        <a:lumMod val="60000"/>
+                        <a:lumOff val="40000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst>
+                      <a:glow rad="63500">
+                        <a:schemeClr val="accent2">
+                          <a:satMod val="175000"/>
+                          <a:alpha val="25000"/>
+                        </a:schemeClr>
+                      </a:glow>
+                    </a:effectLst>
+                  </c:spPr>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="lt1">
+                              <a:lumMod val="75000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="r"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="lt1">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Produksi Telur Data'!$A$2:$B$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="6"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>05-Jun</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>07-Jun</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>09-Jun</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>12-Jun</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>14-Jun</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>16-Jun</c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Produksi Telur Data'!$D$2:$D$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>60</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>62</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>63</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>66</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>63</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-3FDB-4687-A9DE-BDDA83D550B4}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Produksi Telur Data'!$E$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>bh1750-lx</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="22225" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:glow rad="139700">
+                      <a:schemeClr val="accent3">
+                        <a:satMod val="175000"/>
+                        <a:alpha val="14000"/>
+                      </a:schemeClr>
+                    </a:glow>
+                  </a:effectLst>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="4"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3">
+                        <a:lumMod val="60000"/>
+                        <a:lumOff val="40000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst>
+                      <a:glow rad="63500">
+                        <a:schemeClr val="accent3">
+                          <a:satMod val="175000"/>
+                          <a:alpha val="25000"/>
+                        </a:schemeClr>
+                      </a:glow>
+                    </a:effectLst>
+                  </c:spPr>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="lt1">
+                              <a:lumMod val="75000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="r"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="lt1">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Produksi Telur Data'!$A$2:$B$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="6"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>05-Jun</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>07-Jun</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>09-Jun</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>12-Jun</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>14-Jun</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>16-Jun</c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Produksi Telur Data'!$E$2:$E$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>5118</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>7700</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3268</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4742</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5655</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>4020</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-3FDB-4687-A9DE-BDDA83D550B4}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Produksi Telur Data'!$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>telur</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="22225" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:glow rad="139700">
+                      <a:schemeClr val="accent5">
+                        <a:satMod val="175000"/>
+                        <a:alpha val="14000"/>
+                      </a:schemeClr>
+                    </a:glow>
+                  </a:effectLst>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="4"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent5">
+                        <a:lumMod val="60000"/>
+                        <a:lumOff val="40000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst>
+                      <a:glow rad="63500">
+                        <a:schemeClr val="accent5">
+                          <a:satMod val="175000"/>
+                          <a:alpha val="25000"/>
+                        </a:schemeClr>
+                      </a:glow>
+                    </a:effectLst>
+                  </c:spPr>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="lt1">
+                              <a:lumMod val="75000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="r"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="lt1">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Produksi Telur Data'!$A$2:$B$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="6"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>09:00</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>05-Jun</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>07-Jun</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>09-Jun</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>12-Jun</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>14-Jun</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>16-Jun</c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Produksi Telur Data'!$G$2:$G$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>11000</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>6000</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2000</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2000</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2000</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>250</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-3FDB-4687-A9DE-BDDA83D550B4}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1846123872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="high"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1846133952"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1846133952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1846123872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
               <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
@@ -7279,7 +9158,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -28328,7 +30207,87 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors19.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors20.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -32631,6 +34590,509 @@
 </file>
 
 <file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -33179,7 +35641,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style19.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -34227,6 +36689,555 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style20.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -37798,8 +40809,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="4827144"/>
-              <a:ext cx="4572000" cy="2775858"/>
+              <a:off x="0" y="4770538"/>
+              <a:ext cx="4572000" cy="2743201"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -38369,6 +41380,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>603449</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>31195</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>314082</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>25795</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5985AC0-C740-B82A-4A7D-FC99A1025EEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02F8E6B5-230D-9D6D-C59B-58763470BD72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -38714,8 +41797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AG71" sqref="AG71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -40035,27 +43118,27 @@
         <v>51</v>
       </c>
       <c r="I23" s="9">
-        <f>AVERAGE(I2:I21)</f>
+        <f t="shared" ref="I23:N23" si="6">AVERAGE(I2:I21)</f>
         <v>-0.12000000000000011</v>
       </c>
       <c r="J23">
-        <f>AVERAGE(J2:J21)</f>
+        <f t="shared" si="6"/>
         <v>-3.55</v>
       </c>
       <c r="K23">
-        <f>AVERAGE(K2:K21)</f>
+        <f t="shared" si="6"/>
         <v>-9173.2000000000007</v>
       </c>
       <c r="L23" s="5">
-        <f>AVERAGE(L2:L21)</f>
+        <f t="shared" si="6"/>
         <v>-3.5288000624746152E-3</v>
       </c>
       <c r="M23" s="10">
-        <f>AVERAGE(M2:M21)</f>
+        <f t="shared" si="6"/>
         <v>-5.2595144374515526E-2</v>
       </c>
       <c r="N23" s="10">
-        <f>AVERAGE(N2:N21)</f>
+        <f t="shared" si="6"/>
         <v>-0.60928632929819393</v>
       </c>
     </row>
@@ -40064,27 +43147,27 @@
         <v>52</v>
       </c>
       <c r="I24" s="9">
-        <f>MAX(I2:I21)</f>
+        <f t="shared" ref="I24:N24" si="7">MAX(I2:I21)</f>
         <v>2.3999999999999986</v>
       </c>
       <c r="J24">
-        <f>MAX(J2:J21)</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="K24">
-        <f>MAX(K2:K21)</f>
+        <f t="shared" si="7"/>
         <v>-2363</v>
       </c>
       <c r="L24" s="10">
-        <f>MAX(L2:L21)</f>
+        <f t="shared" si="7"/>
         <v>7.2847682119205281E-2</v>
       </c>
       <c r="M24" s="10">
-        <f>MAX(M2:M21)</f>
+        <f t="shared" si="7"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N24" s="10">
-        <f>MAX(N2:N21)</f>
+        <f t="shared" si="7"/>
         <v>-0.43783583472299425</v>
       </c>
     </row>
@@ -40093,27 +43176,27 @@
         <v>53</v>
       </c>
       <c r="I25" s="9">
-        <f>MIN(I2:I21)</f>
+        <f t="shared" ref="I25:N25" si="8">MIN(I2:I21)</f>
         <v>-1.6999999999999957</v>
       </c>
       <c r="J25">
-        <f>MIN(J2:J21)</f>
+        <f t="shared" si="8"/>
         <v>-13</v>
       </c>
       <c r="K25">
-        <f>MIN(K2:K21)</f>
+        <f t="shared" si="8"/>
         <v>-29165</v>
       </c>
       <c r="L25" s="10">
-        <f>MIN(L2:L21)</f>
+        <f t="shared" si="8"/>
         <v>-4.871060171919759E-2</v>
       </c>
       <c r="M25" s="10">
-        <f>MIN(M2:M21)</f>
+        <f t="shared" si="8"/>
         <v>-0.17808219178082191</v>
       </c>
       <c r="N25" s="10">
-        <f>MIN(N2:N21)</f>
+        <f t="shared" si="8"/>
         <v>-0.64441883437602898</v>
       </c>
     </row>

</xml_diff>